<commit_message>
Newest project plan + Sourcing Excel + Bill of Materials
</commit_message>
<xml_diff>
--- a/Group_7_Gantt_ProjectPlan.xlsx
+++ b/Group_7_Gantt_ProjectPlan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{B01A847B-9DA7-4D15-B134-F95F98B5E651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C634F09D-FD2E-498A-A631-09B0E822830C}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{B01A847B-9DA7-4D15-B134-F95F98B5E651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A182E028-CD5D-420C-8130-0CA4EA645D9E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12195" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t>About This Template</t>
   </si>
@@ -241,6 +241,54 @@
   </si>
   <si>
     <t>Sub-WP Leader</t>
+  </si>
+  <si>
+    <t>MS1</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>Hardware Design finished</t>
+  </si>
+  <si>
+    <t>MS2</t>
+  </si>
+  <si>
+    <t>MS3</t>
+  </si>
+  <si>
+    <t>MS4</t>
+  </si>
+  <si>
+    <t>Software Base function done</t>
+  </si>
+  <si>
+    <t>Software Full function done</t>
+  </si>
+  <si>
+    <t>HW/SW Integration done</t>
+  </si>
+  <si>
+    <t>MS5</t>
+  </si>
+  <si>
+    <t>Project delivered</t>
+  </si>
+  <si>
+    <t>01.03.19</t>
+  </si>
+  <si>
+    <t>23.02.19</t>
+  </si>
+  <si>
+    <t>01.04.19</t>
+  </si>
+  <si>
+    <t>14.04.19</t>
+  </si>
+  <si>
+    <t>21.04.19</t>
   </si>
 </sst>
 </file>
@@ -817,7 +865,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -950,24 +998,6 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="8" applyFill="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyBorder="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="5" borderId="3" xfId="9" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="5" borderId="4" xfId="9" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="15" fillId="5" borderId="0" xfId="9" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1016,6 +1046,33 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="5" borderId="3" xfId="9" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="5" borderId="4" xfId="9" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Date" xfId="9" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
@@ -1033,6 +1090,35 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1147,35 +1233,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1418,7 +1475,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="23"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="42"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1446,7 +1503,7 @@
                   <a14:compatExt spid="_x0000_s6150"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1477,14 +1534,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Milestones" displayName="Milestones" ref="B6:G31" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Milestones" displayName="Milestones" ref="B6:G31" totalsRowShown="0" headerRowDxfId="1">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description"/>
     <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To"/>
     <tableColumn id="4" xr3:uid="{A60A6524-18F0-48B7-BB3C-2F4A35799FF7}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{59612C1F-9AAB-483B-A6A5-3563E9D77941}" name="Start"/>
     <tableColumn id="6" xr3:uid="{012C59F1-49D4-4A67-B8DD-855C6581FD6A}" name="No. Days"/>
-    <tableColumn id="7" xr3:uid="{6579BC2A-C93E-4CF3-BFD9-2110C3BCFE42}" name="Estimated Effort (hours)" dataDxfId="8" dataCellStyle="Dezimal [0]"/>
+    <tableColumn id="7" xr3:uid="{6579BC2A-C93E-4CF3-BFD9-2110C3BCFE42}" name="Estimated Effort (hours)" dataDxfId="0" dataCellStyle="Dezimal [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1758,10 +1815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB0E4BA-159D-47D5-849F-E373F41CDE92}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,237 +1832,306 @@
   <sheetData>
     <row r="1" spans="2:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="74"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="67"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="61"/>
+      <c r="C4" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="66" t="s">
+      <c r="D4" s="57"/>
+      <c r="E4" s="60" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
-      <c r="C5" s="63" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="66" t="s">
+      <c r="D5" s="57"/>
+      <c r="E5" s="60" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="67"/>
-      <c r="C6" s="63" t="s">
+      <c r="B6" s="61"/>
+      <c r="C6" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="66" t="s">
+      <c r="D6" s="57"/>
+      <c r="E6" s="60" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="75"/>
-      <c r="C7" s="72" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="76" t="s">
+      <c r="D7" s="66"/>
+      <c r="E7" s="70" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="66"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="67"/>
-      <c r="C9" s="63" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="66" t="s">
+      <c r="D9" s="57"/>
+      <c r="E9" s="60" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="67"/>
-      <c r="C10" s="63" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="66" t="s">
+      <c r="D10" s="57"/>
+      <c r="E10" s="60" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="67"/>
-      <c r="C11" s="63" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="66" t="s">
+      <c r="D11" s="57"/>
+      <c r="E11" s="60" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="67"/>
-      <c r="C12" s="63" t="s">
+      <c r="B12" s="61"/>
+      <c r="C12" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="66" t="s">
+      <c r="D12" s="57"/>
+      <c r="E12" s="60" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71" t="s">
+      <c r="C13" s="65"/>
+      <c r="D13" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="74"/>
+      <c r="E13" s="68"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="67"/>
-      <c r="C14" s="63" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="66" t="s">
+      <c r="D14" s="57"/>
+      <c r="E14" s="60" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="67"/>
-      <c r="C15" s="63" t="s">
+      <c r="B15" s="61"/>
+      <c r="C15" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="66" t="s">
+      <c r="D15" s="57"/>
+      <c r="E15" s="60" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="67"/>
-      <c r="C16" s="63" t="s">
+      <c r="B16" s="61"/>
+      <c r="C16" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="66" t="s">
+      <c r="D16" s="57"/>
+      <c r="E16" s="60" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="67"/>
-      <c r="C17" s="63" t="s">
+      <c r="B17" s="61"/>
+      <c r="C17" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="66" t="s">
+      <c r="D17" s="57"/>
+      <c r="E17" s="60" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="75"/>
-      <c r="C18" s="72" t="s">
+      <c r="B18" s="69"/>
+      <c r="C18" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="76" t="s">
+      <c r="D18" s="66"/>
+      <c r="E18" s="70" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65" t="s">
+      <c r="C19" s="59"/>
+      <c r="D19" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="66"/>
+      <c r="E19" s="60"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="67"/>
-      <c r="C20" s="63" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="63"/>
-      <c r="E20" s="66" t="s">
+      <c r="D20" s="57"/>
+      <c r="E20" s="60" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="67"/>
-      <c r="C21" s="63" t="s">
+      <c r="B21" s="61"/>
+      <c r="C21" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="63"/>
-      <c r="E21" s="66" t="s">
+      <c r="D21" s="57"/>
+      <c r="E21" s="60" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71" t="s">
+      <c r="C22" s="65"/>
+      <c r="D22" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="74"/>
+      <c r="E22" s="68"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="67"/>
-      <c r="C23" s="62" t="s">
+      <c r="B23" s="61"/>
+      <c r="C23" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="66" t="s">
+      <c r="D23" s="56"/>
+      <c r="E23" s="60" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="68"/>
-      <c r="C24" s="69" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="70" t="s">
+      <c r="D24" s="63"/>
+      <c r="E24" s="64" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B28" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="73"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="67"/>
+      <c r="C29" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="61"/>
+      <c r="C30" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="61"/>
+      <c r="C31" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="61"/>
+      <c r="C32" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="69"/>
+      <c r="C33" s="82" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="70" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2020,8 +2146,8 @@
   </sheetPr>
   <dimension ref="A1:BL35"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C29"/>
+    <sheetView showGridLines="0" showRuler="0" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AX22" sqref="AX22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2059,15 +2185,15 @@
       <c r="B2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54">
+      <c r="D2" s="75"/>
+      <c r="E2" s="76">
         <v>43474</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="58"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="52"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
@@ -2082,12 +2208,12 @@
       <c r="B3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="75"/>
       <c r="E3" s="39">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I3" s="50"/>
       <c r="J3" s="51"/>
@@ -2095,15 +2221,16 @@
       <c r="L3" s="51"/>
       <c r="M3" s="51"/>
       <c r="N3" s="50"/>
+      <c r="AG3" s="37"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="40">
         <v>2</v>
       </c>
@@ -2134,7 +2261,7 @@
       <c r="V4" s="17"/>
       <c r="W4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(W5,"mmmm")=P4,TEXT(W5,"mmmm")=I4),"",TEXT(W5,"mmmm"))</f>
-        <v/>
+        <v>March</v>
       </c>
       <c r="X4" s="17"/>
       <c r="Y4" s="17"/>
@@ -2154,7 +2281,7 @@
       <c r="AJ4" s="17"/>
       <c r="AK4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(AK5,"mmmm")=AD4,TEXT(AK5,"mmmm")=W4,TEXT(AK5,"mmmm")=P4,TEXT(AK5,"mmmm")=I4),"",TEXT(AK5,"mmmm"))</f>
-        <v>March</v>
+        <v/>
       </c>
       <c r="AL4" s="17"/>
       <c r="AM4" s="17"/>
@@ -2174,7 +2301,7 @@
       <c r="AX4" s="17"/>
       <c r="AY4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(AY5,"mmmm")=AR4,TEXT(AY5,"mmmm")=AK4,TEXT(AY5,"mmmm")=AD4,TEXT(AY5,"mmmm")=W4),"",TEXT(AY5,"mmmm"))</f>
-        <v/>
+        <v>April</v>
       </c>
       <c r="AZ4" s="17"/>
       <c r="BA4" s="17"/>
@@ -2201,275 +2328,275 @@
       <c r="H5" s="35"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>43497</v>
+        <v>43516</v>
       </c>
       <c r="J5" s="45">
         <f ca="1">I5+1</f>
-        <v>43498</v>
+        <v>43517</v>
       </c>
       <c r="K5" s="42">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>43499</v>
+        <v>43518</v>
       </c>
       <c r="L5" s="42">
         <f ca="1">K5+1</f>
-        <v>43500</v>
+        <v>43519</v>
       </c>
       <c r="M5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43501</v>
+        <v>43520</v>
       </c>
       <c r="N5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43502</v>
+        <v>43521</v>
       </c>
       <c r="O5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43503</v>
+        <v>43522</v>
       </c>
       <c r="P5" s="42">
         <f ca="1">O5+1</f>
-        <v>43504</v>
+        <v>43523</v>
       </c>
       <c r="Q5" s="42">
         <f ca="1">P5+1</f>
-        <v>43505</v>
+        <v>43524</v>
       </c>
       <c r="R5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43506</v>
+        <v>43525</v>
       </c>
       <c r="S5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43507</v>
+        <v>43526</v>
       </c>
       <c r="T5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43508</v>
+        <v>43527</v>
       </c>
       <c r="U5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43509</v>
+        <v>43528</v>
       </c>
       <c r="V5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43510</v>
+        <v>43529</v>
       </c>
       <c r="W5" s="42">
         <f ca="1">V5+1</f>
-        <v>43511</v>
+        <v>43530</v>
       </c>
       <c r="X5" s="42">
         <f ca="1">W5+1</f>
-        <v>43512</v>
+        <v>43531</v>
       </c>
       <c r="Y5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43513</v>
+        <v>43532</v>
       </c>
       <c r="Z5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43514</v>
+        <v>43533</v>
       </c>
       <c r="AA5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43515</v>
+        <v>43534</v>
       </c>
       <c r="AB5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43516</v>
+        <v>43535</v>
       </c>
       <c r="AC5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43517</v>
+        <v>43536</v>
       </c>
       <c r="AD5" s="42">
         <f ca="1">AC5+1</f>
-        <v>43518</v>
+        <v>43537</v>
       </c>
       <c r="AE5" s="42">
         <f ca="1">AD5+1</f>
-        <v>43519</v>
+        <v>43538</v>
       </c>
       <c r="AF5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43520</v>
+        <v>43539</v>
       </c>
       <c r="AG5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43521</v>
+        <v>43540</v>
       </c>
       <c r="AH5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43522</v>
+        <v>43541</v>
       </c>
       <c r="AI5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43523</v>
+        <v>43542</v>
       </c>
       <c r="AJ5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43524</v>
+        <v>43543</v>
       </c>
       <c r="AK5" s="42">
         <f ca="1">AJ5+1</f>
-        <v>43525</v>
+        <v>43544</v>
       </c>
       <c r="AL5" s="42">
         <f ca="1">AK5+1</f>
-        <v>43526</v>
+        <v>43545</v>
       </c>
       <c r="AM5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43527</v>
+        <v>43546</v>
       </c>
       <c r="AN5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43528</v>
+        <v>43547</v>
       </c>
       <c r="AO5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43529</v>
+        <v>43548</v>
       </c>
       <c r="AP5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43530</v>
+        <v>43549</v>
       </c>
       <c r="AQ5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43531</v>
+        <v>43550</v>
       </c>
       <c r="AR5" s="42">
         <f ca="1">AQ5+1</f>
-        <v>43532</v>
+        <v>43551</v>
       </c>
       <c r="AS5" s="42">
         <f ca="1">AR5+1</f>
-        <v>43533</v>
+        <v>43552</v>
       </c>
       <c r="AT5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43534</v>
+        <v>43553</v>
       </c>
       <c r="AU5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43535</v>
+        <v>43554</v>
       </c>
       <c r="AV5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43536</v>
+        <v>43555</v>
       </c>
       <c r="AW5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43537</v>
+        <v>43556</v>
       </c>
       <c r="AX5" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>43538</v>
+        <v>43557</v>
       </c>
       <c r="AY5" s="42">
         <f ca="1">AX5+1</f>
-        <v>43539</v>
+        <v>43558</v>
       </c>
       <c r="AZ5" s="42">
         <f ca="1">AY5+1</f>
-        <v>43540</v>
+        <v>43559</v>
       </c>
       <c r="BA5" s="42">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>43541</v>
+        <v>43560</v>
       </c>
       <c r="BB5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43542</v>
+        <v>43561</v>
       </c>
       <c r="BC5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43543</v>
+        <v>43562</v>
       </c>
       <c r="BD5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43544</v>
+        <v>43563</v>
       </c>
       <c r="BE5" s="42">
         <f t="shared" ca="1" si="1"/>
-        <v>43545</v>
+        <v>43564</v>
       </c>
       <c r="BF5" s="42">
         <f ca="1">BE5+1</f>
-        <v>43546</v>
+        <v>43565</v>
       </c>
       <c r="BG5" s="42">
         <f ca="1">BF5+1</f>
-        <v>43547</v>
+        <v>43566</v>
       </c>
       <c r="BH5" s="42">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>43548</v>
+        <v>43567</v>
       </c>
       <c r="BI5" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>43549</v>
+        <v>43568</v>
       </c>
       <c r="BJ5" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>43550</v>
+        <v>43569</v>
       </c>
       <c r="BK5" s="42">
         <f t="shared" ca="1" si="2"/>
-        <v>43551</v>
+        <v>43570</v>
       </c>
       <c r="BL5" s="44">
         <f t="shared" ca="1" si="2"/>
-        <v>43552</v>
+        <v>43571</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="55" t="s">
         <v>45</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="43" t="str">
         <f ca="1">LEFT(TEXT(I5,"ddd"),1)</f>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="J6" s="46" t="str">
         <f ca="1">LEFT(TEXT(J5,"ddd"),1)</f>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="K6" s="48" t="str">
         <f ca="1">LEFT(TEXT(K5,"ddd"),1)</f>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="L6" s="47" t="str">
         <f t="shared" ref="L6:AN6" ca="1" si="3">LEFT(TEXT(L5,"ddd"),1)</f>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="M6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="N6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="O6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2477,27 +2604,27 @@
       </c>
       <c r="P6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="Q6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="R6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="S6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="T6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="U6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="V6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2505,27 +2632,27 @@
       </c>
       <c r="W6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="X6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="Y6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="Z6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AA6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AB6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AC6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2533,27 +2660,27 @@
       </c>
       <c r="AD6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AE6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AF6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AG6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AH6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AI6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AJ6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2561,27 +2688,27 @@
       </c>
       <c r="AK6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AL6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AM6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AN6" s="47" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AO6" s="47" t="str">
         <f t="shared" ref="AO6:BL6" ca="1" si="4">LEFT(TEXT(AO5,"ddd"),1)</f>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AP6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AQ6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2589,27 +2716,27 @@
       </c>
       <c r="AR6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AS6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AT6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="AU6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AV6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AW6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="AX6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2617,27 +2744,27 @@
       </c>
       <c r="AY6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="AZ6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BA6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BB6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BC6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BD6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="BE6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2645,27 +2772,27 @@
       </c>
       <c r="BF6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>W</v>
       </c>
       <c r="BG6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BH6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>F</v>
       </c>
       <c r="BI6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BJ6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BK6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>W</v>
+        <v>M</v>
       </c>
       <c r="BL6" s="47" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -7643,7 +7770,7 @@
     </row>
     <row r="34" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="6"/>
-      <c r="G34" s="59">
+      <c r="G34" s="53">
         <f>SUM(G10:G29)</f>
         <v>525</v>
       </c>
@@ -7662,7 +7789,7 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D8 D30:D31 D10:D26">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7676,22 +7803,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BL8 I30:BL31 I10:BL26">
-    <cfRule type="expression" dxfId="6" priority="90">
+    <cfRule type="expression" dxfId="8" priority="94">
       <formula>I$5&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL8 I10:BL31">
-    <cfRule type="expression" dxfId="5" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
       <formula>AND(I$5&gt;=$E7+1,I$5&lt;=$E7+$F7-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL6">
-    <cfRule type="expression" dxfId="4" priority="13">
+    <cfRule type="expression" dxfId="6" priority="17">
       <formula>I$5&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D28">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7705,12 +7832,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:BL28">
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="5" priority="15">
       <formula>I$5&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7724,12 +7851,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29:BL29">
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>I$5&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7743,12 +7870,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BL9">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>I$5&lt;=Today</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BL9">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>AND(I$5&gt;=$E9+1,I$5&lt;=$E9+$F9-2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7815,7 +7942,52 @@
           <xm:sqref>D6:D8 D30:D31 D10:D26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="14" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
+          <x14:cfRule type="dataBar" id="{8CB8FDBF-7DD4-4DBA-9320-09A549E2E8F0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D27:D28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4E24484B-F10A-4421-8B29-24D5C55C59D0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{54E51C5B-7875-4E25-AFEA-7DB3D15E769D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="18" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
             <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7834,7 +8006,7 @@
           <xm:sqref>F4:G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="111" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
+          <x14:cfRule type="iconSet" priority="115" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7853,22 +8025,7 @@
           <xm:sqref>I30:BL31 I7:BL8 I10:BL26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{8CB8FDBF-7DD4-4DBA-9320-09A549E2E8F0}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D27:D28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{90BD489B-80C0-4208-8DA7-CC62090899D6}">
+          <x14:cfRule type="iconSet" priority="16" id="{90BD489B-80C0-4208-8DA7-CC62090899D6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7887,22 +8044,7 @@
           <xm:sqref>I27:BL28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4E24484B-F10A-4421-8B29-24D5C55C59D0}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D29</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{A7EDCFF4-D5B9-49BF-83EF-599FF2F0EE38}">
+          <x14:cfRule type="iconSet" priority="12" id="{A7EDCFF4-D5B9-49BF-83EF-599FF2F0EE38}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7921,22 +8063,7 @@
           <xm:sqref>I29:BL29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{54E51C5B-7875-4E25-AFEA-7DB3D15E769D}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{6618B2CE-7C4B-4D94-A746-A489A36B6681}">
+          <x14:cfRule type="iconSet" priority="8" id="{6618B2CE-7C4B-4D94-A746-A489A36B6681}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7953,6 +8080,25 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I9:BL9</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{E502F0AB-920E-4D2A-90B2-F8D61B30FD2D}">
+            <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="1"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>AG3</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>